<commit_message>
Updating Volontari/Mezzi/Volontari attesi/Mezzi attesi
</commit_message>
<xml_diff>
--- a/tables/xls/it/60_Volontari.xlsx
+++ b/tables/xls/it/60_Volontari.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="89">
   <si>
     <t>ORGANIZZAZIONE</t>
   </si>
@@ -33,6 +33,9 @@
     <t>CODICE FISCALE</t>
   </si>
   <si>
+    <t>DATA DI NASCITA</t>
+  </si>
+  <si>
     <t>MANSIONE</t>
   </si>
   <si>
@@ -90,6 +93,9 @@
     <t>NOTE</t>
   </si>
   <si>
+    <t>NOME CAMPO</t>
+  </si>
+  <si>
     <t>Sequenza</t>
   </si>
   <si>
@@ -180,10 +186,13 @@
     <t>autofocus</t>
   </si>
   <si>
+    <t>Data</t>
+  </si>
+  <si>
     <t>Testo - Elenco di valori</t>
   </si>
   <si>
-    <t>OPERATORE LOGISTICO (GENERICO),OPERATORE LOGISTICO (INSACCHETTAMENTO),OPERATORE LOGISTICO (MOTOSEGA),OPERATORE LOGISTICO (MOTOPOMPE),OPERATORE LOGISTICO (SUB),OPERATORE CINOFILO,OPERATORE SEGRETERIA,OPERATORE SALA OPERATIVA,OPERATORE RADIO,OPERATORE NAUTICO,ELETTRICISTA,MURATORE,IDRAULICO,OPERATORE SANITARIO,OPERATORE CUCINA,OPERATORE ANTINCENDIO,OPERATORE A CAVALLO,OPERATORE SUBACQUEO</t>
+    <t>OPERATORE LOGISTICO,OPERATORE IDROGEOLOGICO,OPERATORE MOVIMENTO TERRA,OPERATORE INSACCHETTAMENTO,OPERATORE MOTOSEGA,OPERATORE SUB,OPERATORE CINOFILO,OPERATORE SEGRETERIA,OPERATORE SALA OPERATIVA,OPERATORE RADIO,OPERATORE NAUTICO,ELETTRICISTA,MURATORE,IDRAULICO,OPERATORE SANITARIO,OPERATORE CUCINA,OPERATORE ANTINCENDIO,OPERATORE A CAVALLO,OPERATORE SUBACQUEO</t>
   </si>
   <si>
     <t>IN ATTESA DI SERVIZIO</t>
@@ -234,9 +243,6 @@
     <t>DATA INIZIO ATTEST.</t>
   </si>
   <si>
-    <t>Data</t>
-  </si>
-  <si>
     <t>oggi</t>
   </si>
   <si>
@@ -253,6 +259,9 @@
   </si>
   <si>
     <t>DATA/ORA USCITA</t>
+  </si>
+  <si>
+    <t>${nomecampo}</t>
   </si>
   <si>
     <t>VOLONTARI</t>
@@ -609,7 +618,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:X1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -617,7 +626,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:26">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -689,6 +698,12 @@
       </c>
       <c r="X1" t="s">
         <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -713,7 +728,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:Y25"/>
+  <dimension ref="A1:AA25"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -721,7 +736,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:27">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -794,10 +809,16 @@
       <c r="Y1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:25">
+      <c r="Z1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -815,66 +836,72 @@
         <v>5</v>
       </c>
       <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2">
         <v>6</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>7</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>8</v>
-      </c>
-      <c r="J2">
-        <v>9</v>
       </c>
       <c r="K2">
         <v>9</v>
       </c>
       <c r="L2">
+        <v>9</v>
+      </c>
+      <c r="M2">
         <v>10</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>11</v>
       </c>
-      <c r="N2">
+      <c r="O2">
         <v>12</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>24</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>25</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>29</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>30</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>32</v>
       </c>
-      <c r="T2">
+      <c r="U2">
         <v>33</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>80</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>81</v>
       </c>
-      <c r="W2">
+      <c r="X2">
         <v>90</v>
       </c>
-      <c r="X2">
+      <c r="Y2">
         <v>93</v>
       </c>
-      <c r="Y2">
+      <c r="Z2">
         <v>99</v>
       </c>
-    </row>
-    <row r="3" spans="1:25">
+      <c r="AA2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -898,10 +925,10 @@
         <v>6</v>
       </c>
       <c r="I3" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="J3" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="K3" t="s">
         <v>9</v>
@@ -913,152 +940,164 @@
         <v>11</v>
       </c>
       <c r="N3" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="O3" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="P3" t="s">
         <v>14</v>
       </c>
       <c r="Q3" t="s">
-        <v>67</v>
+        <v>15</v>
       </c>
       <c r="R3" t="s">
-        <v>16</v>
+        <v>70</v>
       </c>
       <c r="S3" t="s">
         <v>17</v>
       </c>
       <c r="T3" t="s">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="U3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="V3" t="s">
         <v>74</v>
       </c>
       <c r="W3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="X3" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K4" t="s">
+        <v>50</v>
+      </c>
+      <c r="L4" t="s">
+        <v>57</v>
+      </c>
+      <c r="M4" t="s">
+        <v>57</v>
+      </c>
+      <c r="N4" t="s">
+        <v>57</v>
+      </c>
+      <c r="O4" t="s">
+        <v>57</v>
+      </c>
+      <c r="P4" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>69</v>
+      </c>
+      <c r="R4" t="s">
+        <v>50</v>
+      </c>
+      <c r="S4" t="s">
+        <v>50</v>
+      </c>
+      <c r="T4" t="s">
+        <v>50</v>
+      </c>
+      <c r="U4" t="s">
+        <v>50</v>
+      </c>
+      <c r="V4" t="s">
+        <v>56</v>
+      </c>
+      <c r="W4" t="s">
+        <v>56</v>
+      </c>
+      <c r="X4" t="s">
         <v>78</v>
       </c>
-      <c r="Y3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" t="s">
-        <v>54</v>
-      </c>
-      <c r="H4" t="s">
-        <v>48</v>
-      </c>
-      <c r="I4" t="s">
-        <v>54</v>
-      </c>
-      <c r="J4" t="s">
-        <v>48</v>
-      </c>
-      <c r="K4" t="s">
-        <v>54</v>
-      </c>
-      <c r="L4" t="s">
-        <v>54</v>
-      </c>
-      <c r="M4" t="s">
-        <v>54</v>
-      </c>
-      <c r="N4" t="s">
-        <v>54</v>
-      </c>
-      <c r="O4" t="s">
-        <v>54</v>
-      </c>
-      <c r="P4" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>48</v>
-      </c>
-      <c r="R4" t="s">
-        <v>48</v>
-      </c>
-      <c r="S4" t="s">
-        <v>48</v>
-      </c>
-      <c r="T4" t="s">
-        <v>48</v>
-      </c>
-      <c r="U4" t="s">
-        <v>72</v>
-      </c>
-      <c r="V4" t="s">
-        <v>72</v>
-      </c>
-      <c r="W4" t="s">
-        <v>76</v>
-      </c>
-      <c r="X4" t="s">
-        <v>76</v>
-      </c>
       <c r="Y4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25">
+        <v>78</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B5"/>
       <c r="C5"/>
       <c r="D5"/>
       <c r="E5"/>
       <c r="F5"/>
-      <c r="G5" t="s">
-        <v>55</v>
-      </c>
-      <c r="H5"/>
-      <c r="I5" t="s">
+      <c r="G5"/>
+      <c r="H5" t="s">
         <v>58</v>
       </c>
-      <c r="J5"/>
-      <c r="K5" t="s">
-        <v>62</v>
-      </c>
+      <c r="I5"/>
+      <c r="J5" t="s">
+        <v>61</v>
+      </c>
+      <c r="K5"/>
       <c r="L5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="M5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="N5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="O5" t="s">
-        <v>62</v>
-      </c>
-      <c r="P5"/>
+        <v>65</v>
+      </c>
+      <c r="P5" t="s">
+        <v>65</v>
+      </c>
       <c r="Q5"/>
       <c r="R5"/>
       <c r="S5"/>
@@ -1068,10 +1107,12 @@
       <c r="W5"/>
       <c r="X5"/>
       <c r="Y5"/>
-    </row>
-    <row r="6" spans="1:25">
+      <c r="Z5"/>
+      <c r="AA5"/>
+    </row>
+    <row r="6" spans="1:27">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B6">
         <v>255</v>
@@ -1095,11 +1136,11 @@
         <v>255</v>
       </c>
       <c r="I6">
+        <v>255</v>
+      </c>
+      <c r="J6">
         <v>1</v>
       </c>
-      <c r="J6">
-        <v>255</v>
-      </c>
       <c r="K6">
         <v>255</v>
       </c>
@@ -1145,87 +1186,99 @@
       <c r="Y6">
         <v>255</v>
       </c>
-    </row>
-    <row r="7" spans="1:25">
+      <c r="Z6">
+        <v>255</v>
+      </c>
+      <c r="AA6">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="J7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="K7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="M7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="N7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="O7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="P7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="Q7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="R7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="S7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="T7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="U7" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="V7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="W7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="X7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="Y7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25">
+        <v>52</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B8"/>
       <c r="C8"/>
@@ -1233,343 +1286,367 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8"/>
-      <c r="H8" t="s">
-        <v>56</v>
-      </c>
+      <c r="H8"/>
       <c r="I8" t="s">
         <v>59</v>
       </c>
-      <c r="J8"/>
+      <c r="J8" t="s">
+        <v>62</v>
+      </c>
       <c r="K8"/>
       <c r="L8"/>
       <c r="M8"/>
       <c r="N8"/>
-      <c r="O8" t="s">
-        <v>59</v>
-      </c>
-      <c r="P8"/>
+      <c r="O8"/>
+      <c r="P8" t="s">
+        <v>62</v>
+      </c>
       <c r="Q8"/>
-      <c r="R8" t="s">
-        <v>68</v>
-      </c>
+      <c r="R8"/>
       <c r="S8" t="s">
-        <v>69</v>
-      </c>
-      <c r="T8"/>
-      <c r="U8" t="s">
-        <v>73</v>
-      </c>
-      <c r="V8"/>
-      <c r="W8" t="s">
-        <v>77</v>
-      </c>
-      <c r="X8"/>
+        <v>71</v>
+      </c>
+      <c r="T8" t="s">
+        <v>72</v>
+      </c>
+      <c r="U8"/>
+      <c r="V8" t="s">
+        <v>75</v>
+      </c>
+      <c r="W8"/>
+      <c r="X8" t="s">
+        <v>79</v>
+      </c>
       <c r="Y8"/>
-    </row>
-    <row r="9" spans="1:25">
+      <c r="Z8"/>
+      <c r="AA8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="J9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="K9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="M9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="N9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="O9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="P9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="Q9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="R9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="S9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="T9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="U9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="V9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="W9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="X9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="Y9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25">
+        <v>52</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="I10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="J10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="K10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="L10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="M10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="N10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="O10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="P10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="Q10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="R10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="S10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="T10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="U10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="V10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="W10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="X10" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="Y10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25">
+        <v>51</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C11"/>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E11" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F11" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" t="s">
-        <v>50</v>
-      </c>
-      <c r="H11"/>
-      <c r="I11" t="s">
-        <v>50</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="G11"/>
+      <c r="H11" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11"/>
       <c r="J11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="K11" t="s">
-        <v>50</v>
-      </c>
-      <c r="L11"/>
+        <v>52</v>
+      </c>
+      <c r="L11" t="s">
+        <v>52</v>
+      </c>
       <c r="M11"/>
       <c r="N11"/>
-      <c r="O11" t="s">
-        <v>50</v>
-      </c>
-      <c r="P11"/>
+      <c r="O11"/>
+      <c r="P11" t="s">
+        <v>52</v>
+      </c>
       <c r="Q11"/>
-      <c r="R11" t="s">
-        <v>50</v>
-      </c>
+      <c r="R11"/>
       <c r="S11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="T11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="U11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="V11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="W11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="X11" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="Y11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25">
+        <v>52</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA11"/>
+    </row>
+    <row r="12" spans="1:27">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="I12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="J12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="K12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="L12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="M12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="N12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="O12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="P12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="Q12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="R12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="S12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="T12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="U12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="V12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="W12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="X12" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="Y12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25">
+        <v>52</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B13"/>
       <c r="C13"/>
       <c r="D13"/>
       <c r="E13"/>
       <c r="F13" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="G13"/>
       <c r="H13"/>
@@ -1590,61 +1667,67 @@
       <c r="W13"/>
       <c r="X13"/>
       <c r="Y13"/>
-    </row>
-    <row r="14" spans="1:25">
+      <c r="Z13"/>
+      <c r="AA13"/>
+    </row>
+    <row r="14" spans="1:27">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E14" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F14" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G14" t="s">
-        <v>52</v>
-      </c>
-      <c r="H14"/>
-      <c r="I14" t="s">
-        <v>52</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="H14" t="s">
+        <v>54</v>
+      </c>
+      <c r="I14"/>
       <c r="J14" t="s">
-        <v>52</v>
-      </c>
-      <c r="K14"/>
+        <v>54</v>
+      </c>
+      <c r="K14" t="s">
+        <v>54</v>
+      </c>
       <c r="L14"/>
       <c r="M14"/>
       <c r="N14"/>
       <c r="O14"/>
       <c r="P14"/>
-      <c r="Q14" t="s">
-        <v>52</v>
-      </c>
-      <c r="R14"/>
+      <c r="Q14"/>
+      <c r="R14" t="s">
+        <v>54</v>
+      </c>
       <c r="S14"/>
-      <c r="T14" t="s">
-        <v>52</v>
-      </c>
-      <c r="U14"/>
+      <c r="T14"/>
+      <c r="U14" t="s">
+        <v>54</v>
+      </c>
       <c r="V14"/>
       <c r="W14"/>
       <c r="X14"/>
-      <c r="Y14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25">
+      <c r="Y14"/>
+      <c r="Z14" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA14"/>
+    </row>
+    <row r="15" spans="1:27">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
         <v>0</v>
@@ -1664,38 +1747,42 @@
       <c r="G15" t="s">
         <v>5</v>
       </c>
-      <c r="H15"/>
-      <c r="I15" t="s">
-        <v>7</v>
-      </c>
+      <c r="H15" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15"/>
       <c r="J15" t="s">
         <v>8</v>
       </c>
-      <c r="K15"/>
+      <c r="K15" t="s">
+        <v>9</v>
+      </c>
       <c r="L15"/>
       <c r="M15"/>
       <c r="N15"/>
       <c r="O15"/>
       <c r="P15"/>
-      <c r="Q15" t="s">
-        <v>15</v>
-      </c>
-      <c r="R15"/>
+      <c r="Q15"/>
+      <c r="R15" t="s">
+        <v>16</v>
+      </c>
       <c r="S15"/>
-      <c r="T15" t="s">
-        <v>18</v>
-      </c>
-      <c r="U15"/>
+      <c r="T15"/>
+      <c r="U15" t="s">
+        <v>19</v>
+      </c>
       <c r="V15"/>
       <c r="W15"/>
       <c r="X15"/>
-      <c r="Y15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25">
+      <c r="Y15"/>
+      <c r="Z15" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA15"/>
+    </row>
+    <row r="16" spans="1:27">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B16"/>
       <c r="C16"/>
@@ -1704,22 +1791,22 @@
       <c r="F16"/>
       <c r="G16"/>
       <c r="H16"/>
-      <c r="I16" t="s">
-        <v>60</v>
-      </c>
+      <c r="I16"/>
       <c r="J16" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="K16" t="s">
-        <v>63</v>
-      </c>
-      <c r="L16"/>
+        <v>64</v>
+      </c>
+      <c r="L16" t="s">
+        <v>66</v>
+      </c>
       <c r="M16"/>
       <c r="N16"/>
-      <c r="O16" t="s">
-        <v>65</v>
-      </c>
-      <c r="P16"/>
+      <c r="O16"/>
+      <c r="P16" t="s">
+        <v>68</v>
+      </c>
       <c r="Q16"/>
       <c r="R16"/>
       <c r="S16"/>
@@ -1729,83 +1816,85 @@
       <c r="W16"/>
       <c r="X16"/>
       <c r="Y16"/>
-    </row>
-    <row r="17" spans="1:25">
+      <c r="Z16"/>
+      <c r="AA16"/>
+    </row>
+    <row r="17" spans="1:27">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27">
+      <c r="A18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27">
+      <c r="A19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
-      <c r="A18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" t="s">
-        <v>79</v>
-      </c>
-      <c r="C18" t="s">
-        <v>84</v>
-      </c>
-      <c r="D18" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25">
-      <c r="A19" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:27">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B20" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:27">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27">
+      <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27">
+      <c r="A24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27">
+      <c r="A25" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="23" spans="1:25">
-      <c r="A23" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25">
-      <c r="A24" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="1:25">
-      <c r="A25" t="s">
-        <v>47</v>
-      </c>
       <c r="B25" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding "Movimentazione..." as bookmark
</commit_message>
<xml_diff>
--- a/tables/xls/it/60_Volontari.xlsx
+++ b/tables/xls/it/60_Volontari.xlsx
@@ -266,7 +266,7 @@
     <t xml:space="preserve">Volontari</t>
   </si>
   <si>
-    <t xml:space="preserve">Movimentazione risorse</t>
+    <t xml:space="preserve">Movimentazione Volontari</t>
   </si>
   <si>
     <t xml:space="preserve">index.php?dashboard=02</t>
@@ -369,8 +369,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -575,82 +579,82 @@
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="0" t="s">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="0" t="s">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="0" t="s">
+      <c r="Y1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="0" t="s">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -673,1054 +677,1054 @@
   <dimension ref="A1:AA25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="0" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="0" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="0" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="0" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="0" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="I2" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="J2" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="K2" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="L2" s="0" t="n">
+      <c r="L2" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="M2" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="N2" s="0" t="n">
+      <c r="N2" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="O2" s="0" t="n">
+      <c r="O2" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="P2" s="0" t="n">
+      <c r="P2" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="Q2" s="0" t="n">
+      <c r="Q2" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="R2" s="0" t="n">
+      <c r="R2" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="S2" s="0" t="n">
+      <c r="S2" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="T2" s="0" t="n">
+      <c r="T2" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="U2" s="0" t="n">
+      <c r="U2" s="1" t="n">
         <v>33</v>
       </c>
-      <c r="V2" s="0" t="n">
+      <c r="V2" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="W2" s="0" t="n">
+      <c r="W2" s="1" t="n">
         <v>81</v>
       </c>
-      <c r="X2" s="0" t="n">
+      <c r="X2" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="Y2" s="0" t="n">
+      <c r="Y2" s="1" t="n">
         <v>93</v>
       </c>
-      <c r="Z2" s="0" t="n">
+      <c r="Z2" s="1" t="n">
         <v>99</v>
       </c>
-      <c r="AA2" s="0" t="n">
+      <c r="AA2" s="1" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="K3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="0" t="s">
+      <c r="L3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="0" t="s">
+      <c r="M3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="0" t="s">
+      <c r="N3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="0" t="s">
+      <c r="O3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="P3" s="0" t="s">
+      <c r="P3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="Q3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R3" s="0" t="s">
+      <c r="R3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="S3" s="0" t="s">
+      <c r="S3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T3" s="0" t="s">
+      <c r="T3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U3" s="0" t="s">
+      <c r="U3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="V3" s="0" t="s">
+      <c r="V3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="W3" s="0" t="s">
+      <c r="W3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="X3" s="0" t="s">
+      <c r="X3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Y3" s="0" t="s">
+      <c r="Y3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Z3" s="0" t="s">
+      <c r="Z3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AA3" s="0" t="s">
+      <c r="AA3" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="H4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="J4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K4" s="0" t="s">
+      <c r="K4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L4" s="0" t="s">
+      <c r="L4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="M4" s="0" t="s">
+      <c r="M4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="N4" s="0" t="s">
+      <c r="N4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="O4" s="0" t="s">
+      <c r="O4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="P4" s="0" t="s">
+      <c r="P4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q4" s="0" t="s">
+      <c r="Q4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="R4" s="0" t="s">
+      <c r="R4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="S4" s="0" t="s">
+      <c r="S4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="T4" s="0" t="s">
+      <c r="T4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="U4" s="0" t="s">
+      <c r="U4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="V4" s="0" t="s">
+      <c r="V4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="W4" s="0" t="s">
+      <c r="W4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="X4" s="0" t="s">
+      <c r="X4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Y4" s="0" t="s">
+      <c r="Y4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Z4" s="0" t="s">
+      <c r="Z4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AA4" s="0" t="s">
+      <c r="AA4" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="H5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J5" s="0" t="s">
+      <c r="J5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="0" t="s">
+      <c r="L5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M5" s="0" t="s">
+      <c r="M5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N5" s="0" t="s">
+      <c r="N5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O5" s="0" t="s">
+      <c r="O5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="P5" s="0" t="s">
+      <c r="P5" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="0" t="n">
-        <v>255</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>255</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>255</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>255</v>
-      </c>
-      <c r="F6" s="0" t="n">
-        <v>255</v>
-      </c>
-      <c r="G6" s="0" t="n">
-        <v>255</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <v>255</v>
-      </c>
-      <c r="I6" s="0" t="n">
-        <v>255</v>
-      </c>
-      <c r="J6" s="0" t="n">
+      <c r="B6" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="J6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="K6" s="0" t="n">
-        <v>255</v>
-      </c>
-      <c r="L6" s="0" t="n">
-        <v>255</v>
-      </c>
-      <c r="M6" s="0" t="n">
-        <v>255</v>
-      </c>
-      <c r="N6" s="0" t="n">
-        <v>255</v>
-      </c>
-      <c r="O6" s="0" t="n">
-        <v>255</v>
-      </c>
-      <c r="P6" s="0" t="n">
-        <v>255</v>
-      </c>
-      <c r="Q6" s="0" t="n">
-        <v>255</v>
-      </c>
-      <c r="R6" s="0" t="n">
-        <v>255</v>
-      </c>
-      <c r="S6" s="0" t="n">
-        <v>255</v>
-      </c>
-      <c r="T6" s="0" t="n">
-        <v>255</v>
-      </c>
-      <c r="U6" s="0" t="n">
-        <v>255</v>
-      </c>
-      <c r="V6" s="0" t="n">
-        <v>255</v>
-      </c>
-      <c r="W6" s="0" t="n">
-        <v>255</v>
-      </c>
-      <c r="X6" s="0" t="n">
-        <v>255</v>
-      </c>
-      <c r="Y6" s="0" t="n">
-        <v>255</v>
-      </c>
-      <c r="Z6" s="0" t="n">
-        <v>255</v>
-      </c>
-      <c r="AA6" s="0" t="n">
+      <c r="K6" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="L6" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="M6" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="N6" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="O6" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="P6" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="Q6" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="R6" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="S6" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="T6" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="U6" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="V6" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="W6" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="X6" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="Y6" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="Z6" s="1" t="n">
+        <v>255</v>
+      </c>
+      <c r="AA6" s="1" t="n">
         <v>255</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="H7" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="K7" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="L7" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="M7" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="N7" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="O7" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="P7" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q7" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="R7" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="S7" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="T7" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="U7" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="V7" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="W7" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="X7" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y7" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z7" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA7" s="0" t="s">
+      <c r="B7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="R7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA7" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="I8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J8" s="0" t="s">
+      <c r="J8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="P8" s="0" t="s">
+      <c r="P8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="S8" s="0" t="s">
+      <c r="S8" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="T8" s="0" t="s">
+      <c r="T8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="V8" s="0" t="s">
+      <c r="V8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="X8" s="0" t="s">
+      <c r="X8" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AA8" s="0" t="s">
+      <c r="AA8" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="J9" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="K9" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="L9" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="M9" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="N9" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="O9" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="P9" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q9" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="R9" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="S9" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="T9" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="U9" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="V9" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="W9" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="X9" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y9" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z9" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA9" s="0" t="s">
+      <c r="B9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA9" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="I10" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="J10" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="K10" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="L10" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="M10" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="N10" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="O10" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="P10" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q10" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="R10" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="S10" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="T10" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="U10" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="V10" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="W10" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="X10" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y10" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z10" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA10" s="0" t="s">
+      <c r="B10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA10" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F11" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H11" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="K11" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="L11" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="P11" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="S11" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="T11" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="U11" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="V11" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="W11" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="X11" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y11" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z11" s="0" t="s">
+      <c r="H11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z11" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="I12" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="J12" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="K12" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="L12" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="M12" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="N12" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="O12" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="P12" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q12" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="R12" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="S12" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="T12" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="U12" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="V12" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="W12" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="X12" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y12" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z12" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA12" s="0" t="s">
+      <c r="B12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="X12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA12" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="F13" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="F14" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G14" s="0" t="s">
+      <c r="G14" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H14" s="0" t="s">
+      <c r="H14" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="J14" s="0" t="s">
+      <c r="J14" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K14" s="0" t="s">
+      <c r="K14" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="R14" s="0" t="s">
+      <c r="R14" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="U14" s="0" t="s">
+      <c r="U14" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="Z14" s="0" t="s">
+      <c r="Z14" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="F15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G15" s="0" t="s">
+      <c r="G15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H15" s="0" t="s">
+      <c r="H15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J15" s="0" t="s">
+      <c r="J15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K15" s="0" t="s">
+      <c r="K15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="R15" s="0" t="s">
+      <c r="R15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="U15" s="0" t="s">
+      <c r="U15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Z15" s="0" t="s">
+      <c r="Z15" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="J16" s="0" t="s">
+      <c r="J16" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="K16" s="0" t="s">
+      <c r="K16" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="L16" s="0" t="s">
+      <c r="L16" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="P16" s="0" t="s">
+      <c r="P16" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>90</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Aggiornamento schede volontari/mezzi/materiali (enh. recordReadOnlyIfNotNullFields)
</commit_message>
<xml_diff>
--- a/tables/xls/it/60_Volontari.xlsx
+++ b/tables/xls/it/60_Volontari.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="92">
   <si>
     <t>ORGANIZZAZIONE</t>
   </si>
@@ -259,6 +259,9 @@
   </si>
   <si>
     <t>DATA/ORA USCITA</t>
+  </si>
+  <si>
+    <t>SLQP</t>
   </si>
   <si>
     <t>${nomecampo}</t>
@@ -316,15 +319,19 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -632,32 +639,32 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="17" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="5" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="17" bestFit="true" customWidth="true" style="0"/>
-    <col min="6" max="6" width="18" bestFit="true" customWidth="true" style="0"/>
-    <col min="7" max="7" width="10" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="10" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="15" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="11" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="9" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="8" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="5" bestFit="true" customWidth="true" style="0"/>
-    <col min="14" max="14" width="16" bestFit="true" customWidth="true" style="0"/>
-    <col min="15" max="15" width="21" bestFit="true" customWidth="true" style="0"/>
-    <col min="16" max="16" width="23" bestFit="true" customWidth="true" style="0"/>
-    <col min="17" max="17" width="25" bestFit="true" customWidth="true" style="0"/>
-    <col min="18" max="18" width="6" bestFit="true" customWidth="true" style="0"/>
-    <col min="19" max="19" width="15" bestFit="true" customWidth="true" style="0"/>
-    <col min="20" max="20" width="21" bestFit="true" customWidth="true" style="0"/>
-    <col min="21" max="21" width="25" bestFit="true" customWidth="true" style="0"/>
-    <col min="22" max="22" width="23" bestFit="true" customWidth="true" style="0"/>
-    <col min="23" max="23" width="26" bestFit="true" customWidth="true" style="0"/>
-    <col min="24" max="24" width="31" bestFit="true" customWidth="true" style="0"/>
-    <col min="25" max="25" width="5" bestFit="true" customWidth="true" style="0"/>
-    <col min="26" max="26" width="12" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="11.711" bestFit="true" customWidth="true" style="0"/>
+    <col min="3" max="3" width="9.283" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="5.856" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="6" max="6" width="18.71" bestFit="true" customWidth="true" style="0"/>
+    <col min="7" max="7" width="10.569" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="10.569" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="15.282" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="11.711" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="9.283" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="8.141" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="5.856" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="16.425" bestFit="true" customWidth="true" style="0"/>
+    <col min="15" max="15" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="16" max="16" width="23.423" bestFit="true" customWidth="true" style="0"/>
+    <col min="17" max="17" width="25.851" bestFit="true" customWidth="true" style="0"/>
+    <col min="18" max="18" width="6.998" bestFit="true" customWidth="true" style="0"/>
+    <col min="19" max="19" width="15.282" bestFit="true" customWidth="true" style="0"/>
+    <col min="20" max="20" width="21.138" bestFit="true" customWidth="true" style="0"/>
+    <col min="21" max="21" width="25.851" bestFit="true" customWidth="true" style="0"/>
+    <col min="22" max="22" width="23.423" bestFit="true" customWidth="true" style="0"/>
+    <col min="23" max="23" width="26.993" bestFit="true" customWidth="true" style="0"/>
+    <col min="24" max="24" width="31.707" bestFit="true" customWidth="true" style="0"/>
+    <col min="25" max="25" width="5.856" bestFit="true" customWidth="true" style="0"/>
+    <col min="26" max="26" width="12.854" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -741,7 +748,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
@@ -1354,7 +1360,7 @@
       <c r="Y8"/>
       <c r="Z8"/>
       <c r="AA8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:27">
@@ -1700,7 +1706,9 @@
       <c r="V13"/>
       <c r="W13"/>
       <c r="X13"/>
-      <c r="Y13"/>
+      <c r="Y13" t="s">
+        <v>81</v>
+      </c>
       <c r="Z13"/>
       <c r="AA13"/>
     </row>
@@ -1858,7 +1866,7 @@
         <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:27">
@@ -1866,13 +1874,13 @@
         <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C18" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D18" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:27">
@@ -1880,13 +1888,13 @@
         <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C19" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D19" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:27">
@@ -1902,7 +1910,7 @@
         <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:27">
@@ -1934,11 +1942,10 @@
         <v>49</v>
       </c>
       <c r="B25" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
Campo provincia max 2 carattero
</commit_message>
<xml_diff>
--- a/tables/xls/it/60_Volontari.xlsx
+++ b/tables/xls/it/60_Volontari.xlsx
@@ -751,15 +751,6 @@
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-  <tableParts count="0"/>
 </worksheet>
 </file>
 
@@ -1109,20 +1100,12 @@
       <c r="A5" t="s">
         <v>29</v>
       </c>
-      <c r="B5"/>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
-      <c r="G5"/>
       <c r="H5" t="s">
         <v>58</v>
       </c>
-      <c r="I5"/>
       <c r="J5" t="s">
         <v>61</v>
       </c>
-      <c r="K5"/>
       <c r="L5" t="s">
         <v>65</v>
       </c>
@@ -1138,17 +1121,6 @@
       <c r="P5" t="s">
         <v>65</v>
       </c>
-      <c r="Q5"/>
-      <c r="R5"/>
-      <c r="S5"/>
-      <c r="T5"/>
-      <c r="U5"/>
-      <c r="V5"/>
-      <c r="W5"/>
-      <c r="X5"/>
-      <c r="Y5"/>
-      <c r="Z5"/>
-      <c r="AA5"/>
     </row>
     <row r="6" spans="1:27">
       <c r="A6" t="s">
@@ -1158,7 +1130,7 @@
         <v>255</v>
       </c>
       <c r="C6">
-        <v>255</v>
+        <v>2</v>
       </c>
       <c r="D6">
         <v>255</v>
@@ -1320,45 +1292,27 @@
       <c r="A8" t="s">
         <v>32</v>
       </c>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
-      <c r="G8"/>
-      <c r="H8"/>
       <c r="I8" t="s">
         <v>59</v>
       </c>
       <c r="J8" t="s">
         <v>62</v>
       </c>
-      <c r="K8"/>
-      <c r="L8"/>
-      <c r="M8"/>
-      <c r="N8"/>
-      <c r="O8"/>
       <c r="P8" t="s">
         <v>62</v>
       </c>
-      <c r="Q8"/>
-      <c r="R8"/>
       <c r="S8" t="s">
         <v>71</v>
       </c>
       <c r="T8" t="s">
         <v>72</v>
       </c>
-      <c r="U8"/>
       <c r="V8" t="s">
         <v>75</v>
       </c>
-      <c r="W8"/>
       <c r="X8" t="s">
         <v>79</v>
       </c>
-      <c r="Y8"/>
-      <c r="Z8"/>
       <c r="AA8" t="s">
         <v>82</v>
       </c>
@@ -1536,7 +1490,9 @@
       <c r="B11" t="s">
         <v>53</v>
       </c>
-      <c r="C11"/>
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
       <c r="D11" t="s">
         <v>53</v>
       </c>
@@ -1546,11 +1502,9 @@
       <c r="F11" t="s">
         <v>53</v>
       </c>
-      <c r="G11"/>
       <c r="H11" t="s">
         <v>52</v>
       </c>
-      <c r="I11"/>
       <c r="J11" t="s">
         <v>52</v>
       </c>
@@ -1560,14 +1514,9 @@
       <c r="L11" t="s">
         <v>52</v>
       </c>
-      <c r="M11"/>
-      <c r="N11"/>
-      <c r="O11"/>
       <c r="P11" t="s">
         <v>52</v>
       </c>
-      <c r="Q11"/>
-      <c r="R11"/>
       <c r="S11" t="s">
         <v>52</v>
       </c>
@@ -1592,7 +1541,6 @@
       <c r="Z11" t="s">
         <v>52</v>
       </c>
-      <c r="AA11"/>
     </row>
     <row r="12" spans="1:27">
       <c r="A12" t="s">
@@ -1681,36 +1629,12 @@
       <c r="A13" t="s">
         <v>37</v>
       </c>
-      <c r="B13"/>
-      <c r="C13"/>
-      <c r="D13"/>
-      <c r="E13"/>
       <c r="F13" t="s">
         <v>55</v>
       </c>
-      <c r="G13"/>
-      <c r="H13"/>
-      <c r="I13"/>
-      <c r="J13"/>
-      <c r="K13"/>
-      <c r="L13"/>
-      <c r="M13"/>
-      <c r="N13"/>
-      <c r="O13"/>
-      <c r="P13"/>
-      <c r="Q13"/>
-      <c r="R13"/>
-      <c r="S13"/>
-      <c r="T13"/>
-      <c r="U13"/>
-      <c r="V13"/>
-      <c r="W13"/>
-      <c r="X13"/>
       <c r="Y13" t="s">
         <v>81</v>
       </c>
-      <c r="Z13"/>
-      <c r="AA13"/>
     </row>
     <row r="14" spans="1:27">
       <c r="A14" t="s">
@@ -1737,35 +1661,21 @@
       <c r="H14" t="s">
         <v>54</v>
       </c>
-      <c r="I14"/>
       <c r="J14" t="s">
         <v>54</v>
       </c>
       <c r="K14" t="s">
         <v>54</v>
       </c>
-      <c r="L14"/>
-      <c r="M14"/>
-      <c r="N14"/>
-      <c r="O14"/>
-      <c r="P14"/>
-      <c r="Q14"/>
       <c r="R14" t="s">
         <v>54</v>
       </c>
-      <c r="S14"/>
-      <c r="T14"/>
       <c r="U14" t="s">
         <v>54</v>
       </c>
-      <c r="V14"/>
-      <c r="W14"/>
-      <c r="X14"/>
-      <c r="Y14"/>
       <c r="Z14" t="s">
         <v>54</v>
       </c>
-      <c r="AA14"/>
     </row>
     <row r="15" spans="1:27">
       <c r="A15" t="s">
@@ -1792,48 +1702,26 @@
       <c r="H15" t="s">
         <v>6</v>
       </c>
-      <c r="I15"/>
       <c r="J15" t="s">
         <v>8</v>
       </c>
       <c r="K15" t="s">
         <v>9</v>
       </c>
-      <c r="L15"/>
-      <c r="M15"/>
-      <c r="N15"/>
-      <c r="O15"/>
-      <c r="P15"/>
-      <c r="Q15"/>
       <c r="R15" t="s">
         <v>16</v>
       </c>
-      <c r="S15"/>
-      <c r="T15"/>
       <c r="U15" t="s">
         <v>19</v>
       </c>
-      <c r="V15"/>
-      <c r="W15"/>
-      <c r="X15"/>
-      <c r="Y15"/>
       <c r="Z15" t="s">
         <v>24</v>
       </c>
-      <c r="AA15"/>
     </row>
     <row r="16" spans="1:27">
       <c r="A16" t="s">
         <v>40</v>
       </c>
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16"/>
-      <c r="G16"/>
-      <c r="H16"/>
-      <c r="I16"/>
       <c r="J16" t="s">
         <v>63</v>
       </c>
@@ -1843,23 +1731,9 @@
       <c r="L16" t="s">
         <v>66</v>
       </c>
-      <c r="M16"/>
-      <c r="N16"/>
-      <c r="O16"/>
       <c r="P16" t="s">
         <v>68</v>
       </c>
-      <c r="Q16"/>
-      <c r="R16"/>
-      <c r="S16"/>
-      <c r="T16"/>
-      <c r="U16"/>
-      <c r="V16"/>
-      <c r="W16"/>
-      <c r="X16"/>
-      <c r="Y16"/>
-      <c r="Z16"/>
-      <c r="AA16"/>
     </row>
     <row r="17" spans="1:27">
       <c r="A17" t="s">
@@ -1949,14 +1823,5 @@
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>